<commit_message>
fixed reference batch upload
</commit_message>
<xml_diff>
--- a/public/static/ReferenceUploadTemplate.xlsx
+++ b/public/static/ReferenceUploadTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="211"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -146,8 +146,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -157,10 +158,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,7 +605,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" zoomScalePageLayoutView="265" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -629,6 +631,9 @@
       <c r="A2">
         <v>24972641</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -654,6 +659,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -661,8 +667,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>